<commit_message>
Excel as a databse
Excel as a databse
</commit_message>
<xml_diff>
--- a/Different tasks/excel.xlsx
+++ b/Different tasks/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\Documents\Automation Anywhere Files\Automation Anywhere\My Tasks\AutomationAnywhere\Different tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C39502-9D86-490B-B46F-D00041EACD26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5485F1-EF41-42B9-9ED2-FF7E6C1888C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hakuna_matata" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>Phone Number</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>lp090lmer@timep090th.co.uk</t>
+  </si>
+  <si>
+    <t>asda2</t>
+  </si>
+  <si>
+    <t>asfasf3</t>
   </si>
 </sst>
 </file>
@@ -619,7 +625,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -906,7 +912,9 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -942,7 +950,9 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="A18" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>

</xml_diff>